<commit_message>
Mental Health Reform NPA widgets.
</commit_message>
<xml_diff>
--- a/dashboard_loader/infrastructure_npa_uploader/infrastructure_npa.xlsx
+++ b/dashboard_loader/infrastructure_npa_uploader/infrastructure_npa.xlsx
@@ -5,14 +5,12 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Projects" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Milestones" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="Data1" sheetId="3" state="visible" r:id="rId4"/>
-    <sheet name="Data2" sheetId="4" state="visible" r:id="rId5"/>
-    <sheet name="Description" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="Description" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -24,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="76">
   <si>
     <t xml:space="preserve">Project status as at 31 December 2016</t>
   </si>
@@ -229,12 +227,6 @@
     <t xml:space="preserve">  </t>
   </si>
   <si>
-    <t xml:space="preserve">Road and Rail Projects as of November 2015 - Progress of projects, by number</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Road and Rail Projects as of November 2015 - Progress of projects, by proportion of funds</t>
-  </si>
-  <si>
     <t xml:space="preserve">Measure</t>
   </si>
   <si>
@@ -284,15 +276,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="6">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="\$#,##0"/>
-    <numFmt numFmtId="166" formatCode="########\ ###\ ##0.0;\-########\ ###\ ##0.0;\–"/>
-    <numFmt numFmtId="167" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* \-??_-;_-@_-"/>
-    <numFmt numFmtId="168" formatCode="_-* #,##0_-;\-* #,##0_-;_-* \-??_-;_-@_-"/>
-    <numFmt numFmtId="169" formatCode="_-* #,##0.0_-;\-* #,##0.0_-;_-* \-??_-;_-@_-"/>
   </numFmts>
-  <fonts count="15">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -324,54 +312,6 @@
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="16"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="12"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <i val="true"/>
-      <sz val="12"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="FreeSans"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
@@ -433,15 +373,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="167" fontId="12" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="13">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -482,79 +420,15 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="168" fontId="8" fillId="0" borderId="0" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="8" fillId="0" borderId="0" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="169" fontId="8" fillId="0" borderId="0" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -643,14 +517,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="5.69897959183674"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.0459183673469"/>
-    <col collapsed="false" hidden="false" max="5" min="3" style="0" width="15.8826530612245"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="14.9030612244898"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="19.1683673469388"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="18.7551020408163"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="12.780612244898"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="5.53571428571429"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.7142857142857"/>
+    <col collapsed="false" hidden="false" max="5" min="3" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="14.5816326530612"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="18.8979591836735"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="18.4948979591837"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="12.5561224489796"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1015,17 +889,16 @@
   </sheetPr>
   <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B16" activeCellId="0" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.3010204081633"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="94.6275510204082"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.1683673469388"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.8928571428571"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="93.5510204081633"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.8979591836735"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1280,464 +1153,31 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:O11"/>
-  <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L11" activeCellId="0" sqref="L11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="4" min="1" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.5"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="11.3418367346939"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="10" t="s">
-        <v>61</v>
-      </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
-      <c r="J1" s="10"/>
-      <c r="K1" s="10"/>
-      <c r="L1" s="10"/>
-      <c r="M1" s="10"/>
-      <c r="N1" s="10"/>
-      <c r="O1" s="10"/>
-    </row>
-    <row r="2" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="11"/>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12"/>
-      <c r="H2" s="12"/>
-      <c r="I2" s="12"/>
-      <c r="J2" s="12"/>
-      <c r="K2" s="12"/>
-      <c r="L2" s="12"/>
-      <c r="M2" s="12"/>
-      <c r="N2" s="12"/>
-      <c r="O2" s="12"/>
-    </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="12"/>
-      <c r="C3" s="12"/>
-      <c r="D3" s="12"/>
-      <c r="E3" s="12"/>
-      <c r="F3" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="G3" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="H3" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="I3" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="J3" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="K3" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="L3" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="M3" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="N3" s="12"/>
-      <c r="O3" s="12"/>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="14" t="n">
-        <v>2015</v>
-      </c>
-      <c r="B4" s="15"/>
-      <c r="C4" s="15"/>
-      <c r="D4" s="12"/>
-      <c r="E4" s="15"/>
-      <c r="F4" s="16"/>
-      <c r="G4" s="16"/>
-      <c r="H4" s="16"/>
-      <c r="I4" s="16"/>
-      <c r="J4" s="16"/>
-      <c r="K4" s="16"/>
-      <c r="L4" s="16"/>
-      <c r="M4" s="16"/>
-      <c r="N4" s="12"/>
-      <c r="O4" s="12"/>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="17"/>
-      <c r="B5" s="12"/>
-      <c r="C5" s="18"/>
-      <c r="D5" s="12"/>
-      <c r="E5" s="17" t="s">
-        <v>12</v>
-      </c>
-      <c r="F5" s="19" t="n">
-        <v>33</v>
-      </c>
-      <c r="G5" s="19" t="n">
-        <v>16</v>
-      </c>
-      <c r="H5" s="19" t="n">
-        <v>33</v>
-      </c>
-      <c r="I5" s="19" t="n">
-        <v>10</v>
-      </c>
-      <c r="J5" s="19" t="n">
-        <v>10</v>
-      </c>
-      <c r="K5" s="19" t="n">
-        <v>12</v>
-      </c>
-      <c r="L5" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="M5" s="19" t="n">
-        <v>9</v>
-      </c>
-      <c r="N5" s="12"/>
-      <c r="O5" s="12"/>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="17"/>
-      <c r="B6" s="12"/>
-      <c r="C6" s="18"/>
-      <c r="D6" s="12"/>
-      <c r="E6" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="F6" s="19" t="n">
-        <v>32</v>
-      </c>
-      <c r="G6" s="19" t="n">
-        <v>15</v>
-      </c>
-      <c r="H6" s="19" t="n">
-        <v>29</v>
-      </c>
-      <c r="I6" s="19" t="n">
-        <v>8</v>
-      </c>
-      <c r="J6" s="19" t="n">
-        <v>4</v>
-      </c>
-      <c r="K6" s="19" t="n">
-        <v>8</v>
-      </c>
-      <c r="L6" s="19" t="n">
-        <v>1</v>
-      </c>
-      <c r="M6" s="19" t="n">
-        <v>7</v>
-      </c>
-      <c r="N6" s="12"/>
-      <c r="O6" s="12"/>
-    </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="21"/>
-      <c r="B7" s="12"/>
-      <c r="C7" s="18"/>
-      <c r="D7" s="12"/>
-      <c r="E7" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="F7" s="19" t="n">
-        <v>14</v>
-      </c>
-      <c r="G7" s="19" t="n">
-        <v>17</v>
-      </c>
-      <c r="H7" s="19" t="n">
-        <v>38</v>
-      </c>
-      <c r="I7" s="19" t="n">
-        <v>8</v>
-      </c>
-      <c r="J7" s="19" t="n">
-        <v>6</v>
-      </c>
-      <c r="K7" s="19" t="n">
-        <v>8</v>
-      </c>
-      <c r="L7" s="19" t="n">
-        <v>2</v>
-      </c>
-      <c r="M7" s="19" t="n">
-        <v>6</v>
-      </c>
-      <c r="N7" s="12"/>
-      <c r="O7" s="12"/>
-    </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:O1"/>
-  </mergeCells>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:M7"/>
-  <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B17" activeCellId="0" sqref="B17"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
-      <c r="J1" s="10"/>
-      <c r="K1" s="10"/>
-      <c r="L1" s="10"/>
-      <c r="M1" s="10"/>
-    </row>
-    <row r="2" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="11"/>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12"/>
-      <c r="H2" s="12"/>
-      <c r="I2" s="12"/>
-      <c r="J2" s="12"/>
-      <c r="K2" s="12"/>
-      <c r="L2" s="12"/>
-      <c r="M2" s="12"/>
-    </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="14"/>
-      <c r="B3" s="12"/>
-      <c r="C3" s="12"/>
-      <c r="D3" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="E3" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="F3" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="G3" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="H3" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="I3" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="J3" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="K3" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="L3" s="12"/>
-      <c r="M3" s="12"/>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="14" t="n">
-        <v>2015</v>
-      </c>
-      <c r="B4" s="22"/>
-      <c r="C4" s="23"/>
-      <c r="D4" s="18"/>
-      <c r="E4" s="18"/>
-      <c r="F4" s="18"/>
-      <c r="G4" s="18"/>
-      <c r="H4" s="18"/>
-      <c r="I4" s="18"/>
-      <c r="J4" s="12"/>
-      <c r="K4" s="18"/>
-      <c r="L4" s="12"/>
-      <c r="M4" s="12"/>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="24"/>
-      <c r="C5" s="17" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" s="25" t="n">
-        <v>13.7909123964774</v>
-      </c>
-      <c r="E5" s="25" t="n">
-        <v>69.432064767873</v>
-      </c>
-      <c r="F5" s="25" t="n">
-        <v>33.6637115824636</v>
-      </c>
-      <c r="G5" s="25" t="n">
-        <v>5.83903586241792</v>
-      </c>
-      <c r="H5" s="25" t="n">
-        <v>7.09270697532697</v>
-      </c>
-      <c r="I5" s="25" t="n">
-        <v>42.8084954460033</v>
-      </c>
-      <c r="J5" s="25" t="n">
-        <v>0</v>
-      </c>
-      <c r="K5" s="25" t="n">
-        <v>36.2031222896791</v>
-      </c>
-      <c r="L5" s="12"/>
-      <c r="M5" s="12"/>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="18"/>
-      <c r="C6" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="D6" s="25" t="n">
-        <v>73.9199825317824</v>
-      </c>
-      <c r="E6" s="25" t="n">
-        <v>26.2416007885342</v>
-      </c>
-      <c r="F6" s="25" t="n">
-        <v>36.374666574863</v>
-      </c>
-      <c r="G6" s="25" t="n">
-        <v>21.8383099833776</v>
-      </c>
-      <c r="H6" s="25" t="n">
-        <v>83.9404351385008</v>
-      </c>
-      <c r="I6" s="25" t="n">
-        <v>25.8258495627122</v>
-      </c>
-      <c r="J6" s="25" t="n">
-        <v>98.5036340316375</v>
-      </c>
-      <c r="K6" s="25" t="n">
-        <v>35.9564614050304</v>
-      </c>
-      <c r="L6" s="12"/>
-      <c r="M6" s="12"/>
-    </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="18"/>
-      <c r="C7" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="D7" s="25" t="n">
-        <v>12.2891050717403</v>
-      </c>
-      <c r="E7" s="25" t="n">
-        <v>4.32633444359285</v>
-      </c>
-      <c r="F7" s="25" t="n">
-        <v>29.9616218426734</v>
-      </c>
-      <c r="G7" s="25" t="n">
-        <v>72.3226541542044</v>
-      </c>
-      <c r="H7" s="25" t="n">
-        <v>8.96685788617227</v>
-      </c>
-      <c r="I7" s="25" t="n">
-        <v>31.3656549912845</v>
-      </c>
-      <c r="J7" s="25" t="n">
-        <v>1.49636596836255</v>
-      </c>
-      <c r="K7" s="25" t="n">
-        <v>27.8404163052905</v>
-      </c>
-      <c r="L7" s="12"/>
-      <c r="M7" s="12"/>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:M1"/>
-  </mergeCells>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="91.3877551020408"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="90.4438775510204"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1745,12 +1185,12 @@
         <v>22</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>2016</v>
@@ -1758,43 +1198,43 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="35.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B6" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="B5" s="26" t="s">
+    </row>
+    <row r="7" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B7" s="11" t="s">
         <v>70</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="35.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="27" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="27" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B9" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="B8" s="28" t="s">
+    </row>
+    <row r="10" customFormat="false" ht="46.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B10" s="12" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="28" t="s">
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B11" s="12" t="s">
         <v>75</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="46.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="28" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="28" t="s">
-        <v>77</v>
       </c>
     </row>
   </sheetData>

</xml_diff>